<commit_message>
add some position to base
</commit_message>
<xml_diff>
--- a/baza/kawy.xlsx
+++ b/baza/kawy.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" state="visible" r:id="rId2"/>
@@ -288,7 +288,7 @@
     <t xml:space="preserve">Vespa [a] [e] [fresh] [100%] [lokal]</t>
   </si>
   <si>
-    <t xml:space="preserve">Twarda 66, Warszawa</t>
+    <t xml:space="preserve">zamknieta</t>
   </si>
   <si>
     <t xml:space="preserve">Cafe Studio Pl.Politechniki [a] [e] [fresh] [100%] [lokal]</t>
@@ -400,7 +400,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -455,12 +455,6 @@
       <charset val="238"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF1D2129"/>
-      <name val="Inherit"/>
-      <family val="0"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
@@ -481,12 +475,18 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -526,7 +526,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -544,30 +544,46 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="4" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -651,17 +667,17 @@
   </sheetPr>
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="A1:E18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5344129554656"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.6801619433198"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8866396761134"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.1295546558704"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -964,235 +980,235 @@
   </sheetPr>
   <dimension ref="A2:B29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A1:E18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.914979757085"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.8097165991903"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.3441295546559"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.2388663967611"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+    <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+    <row r="3" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+    <row r="4" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="9" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+    <row r="5" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+    <row r="6" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+    <row r="8" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+    <row r="9" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+    <row r="10" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+    <row r="11" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+    <row r="12" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="9" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+    <row r="13" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
         <v>89</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+    <row r="14" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="s">
         <v>91</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+    <row r="15" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
         <v>93</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+    <row r="16" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="11" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
+    <row r="17" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="12" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
+    <row r="18" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
+    <row r="19" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
+    <row r="20" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="13" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
+    <row r="21" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="14" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
+    <row r="22" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="s">
         <v>107</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
+    <row r="23" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7" t="s">
         <v>109</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
+    <row r="24" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="s">
         <v>111</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
+    <row r="25" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="s">
         <v>113</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
+    <row r="26" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7" t="s">
         <v>115</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
+    <row r="27" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="s">
         <v>117</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
+    <row r="28" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="12" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
+    <row r="29" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7" t="s">
         <v>121</v>
       </c>
       <c r="B29" s="0" t="s">
@@ -1222,7 +1238,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E18"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
add text "zamkniete" to opening hours
</commit_message>
<xml_diff>
--- a/baza/kawy.xlsx
+++ b/baza/kawy.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="363">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -465,7 +465,7 @@
     <t xml:space="preserve">https://www.facebook.com/Cafe-Wielicka-125706064110660/</t>
   </si>
   <si>
-    <t xml:space="preserve">CafeART</t>
+    <t xml:space="preserve">CafeART OF CAFE</t>
   </si>
   <si>
     <t xml:space="preserve">Kolejowa 47</t>
@@ -489,22 +489,10 @@
     <t xml:space="preserve">Jerozolimskie 200</t>
   </si>
   <si>
-    <t xml:space="preserve">Coffeece </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Przemysłowa 12</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cophi</t>
   </si>
   <si>
     <t xml:space="preserve">Hoża 58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Czarne Mleko</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dąbrowskiego 68</t>
   </si>
   <si>
     <t xml:space="preserve">DaftCafe Mokotów</t>
@@ -1189,9 +1177,10 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF1D2129"/>
-      <name val="Inherit"/>
-      <family val="0"/>
+      <color rgb="FF800000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1297,10 +1286,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1309,15 +1294,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1399,24 +1388,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S91"/>
+  <dimension ref="A1:S89"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J47" activeCellId="0" sqref="J47"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C43" activeCellId="0" sqref="C43:D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.8623481781376"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.0526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.8906882591093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5627530364372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.1093117408907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.9271255060729"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6032388663968"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="9" min="6" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.83400809716599"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.74898785425101"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="4.52226720647773"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.7773279352227"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="4.49797570850202"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.8178137651822"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1657,7 +1646,7 @@
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="10" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1801,7 +1790,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="11" t="s">
         <v>82</v>
       </c>
       <c r="B26" s="6" t="s">
@@ -1823,46 +1812,46 @@
       <c r="D27" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="F27" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="H27" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="I27" s="13" t="s">
+      <c r="I27" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="J27" s="13" t="s">
+      <c r="J27" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="K27" s="13" t="s">
+      <c r="K27" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="L27" s="13" t="s">
+      <c r="L27" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="M27" s="13" t="s">
+      <c r="M27" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="N27" s="13" t="s">
+      <c r="N27" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="O27" s="13" t="s">
+      <c r="O27" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="P27" s="13" t="s">
+      <c r="P27" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="Q27" s="13" t="s">
+      <c r="Q27" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="R27" s="13" t="s">
+      <c r="R27" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="S27" s="13" t="s">
+      <c r="S27" s="12" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1879,46 +1868,46 @@
       <c r="D28" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="F28" s="13" t="s">
+      <c r="F28" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="G28" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="H28" s="13" t="s">
+      <c r="H28" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="I28" s="13" t="s">
+      <c r="I28" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="J28" s="13" t="s">
+      <c r="J28" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="K28" s="13" t="s">
+      <c r="K28" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="L28" s="13" t="s">
+      <c r="L28" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="M28" s="13" t="s">
+      <c r="M28" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="N28" s="13" t="s">
+      <c r="N28" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="O28" s="13" t="s">
+      <c r="O28" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="P28" s="13" t="s">
+      <c r="P28" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="Q28" s="13" t="s">
+      <c r="Q28" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="R28" s="13" t="s">
+      <c r="R28" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="S28" s="13" t="s">
+      <c r="S28" s="12" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1935,46 +1924,46 @@
       <c r="D29" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="F29" s="13" t="s">
+      <c r="F29" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="G29" s="13" t="s">
+      <c r="G29" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="H29" s="13" t="s">
+      <c r="H29" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="I29" s="13" t="s">
+      <c r="I29" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J29" s="13" t="s">
+      <c r="J29" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="K29" s="13" t="s">
+      <c r="K29" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="L29" s="13" t="s">
+      <c r="L29" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="M29" s="13" t="s">
+      <c r="M29" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="N29" s="13" t="s">
+      <c r="N29" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="O29" s="13" t="s">
+      <c r="O29" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="P29" s="13" t="s">
+      <c r="P29" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="Q29" s="13" t="s">
+      <c r="Q29" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="R29" s="13" t="s">
+      <c r="R29" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="S29" s="13" t="s">
+      <c r="S29" s="12" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1988,46 +1977,46 @@
       <c r="D30" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="F30" s="13" t="s">
+      <c r="F30" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="G30" s="13" t="s">
+      <c r="G30" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="H30" s="13" t="s">
+      <c r="H30" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="I30" s="13" t="s">
+      <c r="I30" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="J30" s="13" t="s">
+      <c r="J30" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="K30" s="13" t="s">
+      <c r="K30" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="L30" s="13" t="s">
+      <c r="L30" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="M30" s="13" t="s">
+      <c r="M30" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="N30" s="13" t="s">
+      <c r="N30" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="O30" s="13" t="s">
+      <c r="O30" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="P30" s="13" t="s">
+      <c r="P30" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="Q30" s="13" t="s">
+      <c r="Q30" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="R30" s="13" t="s">
+      <c r="R30" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="S30" s="13" t="s">
+      <c r="S30" s="12" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2044,46 +2033,46 @@
       <c r="D31" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="F31" s="13" t="s">
+      <c r="F31" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="G31" s="13" t="s">
+      <c r="G31" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="H31" s="13" t="s">
+      <c r="H31" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="I31" s="13" t="s">
+      <c r="I31" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="J31" s="13" t="s">
+      <c r="J31" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="K31" s="13" t="s">
+      <c r="K31" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="L31" s="13" t="s">
+      <c r="L31" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="M31" s="13" t="s">
+      <c r="M31" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="N31" s="13" t="s">
+      <c r="N31" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="O31" s="13" t="s">
+      <c r="O31" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="P31" s="13" t="s">
+      <c r="P31" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="Q31" s="13" t="s">
+      <c r="Q31" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="R31" s="13" t="s">
+      <c r="R31" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="S31" s="13" t="s">
+      <c r="S31" s="12" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2097,46 +2086,46 @@
       <c r="D32" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="F32" s="13" t="s">
+      <c r="F32" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="G32" s="13" t="s">
+      <c r="G32" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="H32" s="13" t="s">
+      <c r="H32" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="I32" s="13" t="s">
+      <c r="I32" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="J32" s="13" t="s">
+      <c r="J32" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="K32" s="13" t="s">
+      <c r="K32" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="L32" s="13" t="s">
+      <c r="L32" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="M32" s="13" t="s">
+      <c r="M32" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="N32" s="13" t="s">
+      <c r="N32" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="O32" s="13" t="s">
+      <c r="O32" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="P32" s="13" t="s">
+      <c r="P32" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="Q32" s="13" t="s">
+      <c r="Q32" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="R32" s="13" t="s">
+      <c r="R32" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="S32" s="13" t="s">
+      <c r="S32" s="12" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2153,46 +2142,46 @@
       <c r="D33" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="F33" s="13" t="s">
+      <c r="F33" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="G33" s="13" t="s">
+      <c r="G33" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="H33" s="13" t="s">
+      <c r="H33" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="I33" s="13" t="s">
+      <c r="I33" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="J33" s="13" t="s">
+      <c r="J33" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="K33" s="13" t="s">
+      <c r="K33" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="L33" s="13" t="s">
+      <c r="L33" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="M33" s="13" t="s">
+      <c r="M33" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="N33" s="13" t="s">
+      <c r="N33" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="O33" s="13" t="s">
+      <c r="O33" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="P33" s="13" t="s">
+      <c r="P33" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="Q33" s="13" t="s">
+      <c r="Q33" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="R33" s="13" t="s">
+      <c r="R33" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="S33" s="13" t="s">
+      <c r="S33" s="12" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2206,46 +2195,46 @@
       <c r="D34" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="F34" s="13" t="s">
+      <c r="F34" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="G34" s="13" t="s">
+      <c r="G34" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="H34" s="13" t="s">
+      <c r="H34" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="I34" s="13" t="s">
+      <c r="I34" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="J34" s="13" t="s">
+      <c r="J34" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="K34" s="13" t="s">
+      <c r="K34" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="L34" s="13" t="s">
+      <c r="L34" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="M34" s="13" t="s">
+      <c r="M34" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="N34" s="13" t="s">
+      <c r="N34" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="O34" s="13" t="s">
+      <c r="O34" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="P34" s="13" t="s">
+      <c r="P34" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="Q34" s="13" t="s">
+      <c r="Q34" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="R34" s="13" t="s">
+      <c r="R34" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="S34" s="13" t="s">
+      <c r="S34" s="12" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2259,46 +2248,46 @@
       <c r="D35" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="F35" s="13" t="s">
+      <c r="F35" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="G35" s="13" t="s">
+      <c r="G35" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="H35" s="13" t="s">
+      <c r="H35" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="I35" s="13" t="s">
+      <c r="I35" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="J35" s="13" t="s">
+      <c r="J35" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="K35" s="13" t="s">
+      <c r="K35" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="L35" s="13" t="s">
+      <c r="L35" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="M35" s="13" t="s">
+      <c r="M35" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="N35" s="13" t="s">
+      <c r="N35" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="O35" s="13" t="s">
+      <c r="O35" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="P35" s="13" t="s">
+      <c r="P35" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="Q35" s="13" t="s">
+      <c r="Q35" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="R35" s="13" t="s">
+      <c r="R35" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="S35" s="13" t="s">
+      <c r="S35" s="12" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2312,46 +2301,46 @@
       <c r="D36" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="F36" s="13" t="s">
+      <c r="F36" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="G36" s="13" t="s">
+      <c r="G36" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="H36" s="13" t="s">
+      <c r="H36" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="I36" s="13" t="s">
+      <c r="I36" s="12" t="s">
         <v>129</v>
       </c>
       <c r="J36" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="K36" s="13" t="s">
+      <c r="K36" s="12" t="s">
         <v>139</v>
       </c>
       <c r="L36" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="M36" s="13" t="s">
+      <c r="M36" s="12" t="s">
         <v>134</v>
       </c>
       <c r="N36" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="O36" s="13" t="s">
+      <c r="O36" s="12" t="s">
         <v>129</v>
       </c>
       <c r="P36" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="Q36" s="13" t="s">
+      <c r="Q36" s="12" t="s">
         <v>129</v>
       </c>
       <c r="R36" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="S36" s="13" t="s">
+      <c r="S36" s="12" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2368,110 +2357,110 @@
       <c r="D37" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="F37" s="13" t="s">
+      <c r="F37" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="G37" s="13" t="s">
+      <c r="G37" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="H37" s="13" t="s">
+      <c r="H37" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="I37" s="13" t="s">
+      <c r="I37" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="J37" s="13" t="s">
+      <c r="J37" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="K37" s="13" t="s">
+      <c r="K37" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="L37" s="13" t="s">
+      <c r="L37" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="M37" s="13" t="s">
+      <c r="M37" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="N37" s="13" t="s">
+      <c r="N37" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="O37" s="13" t="s">
+      <c r="O37" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="P37" s="13" t="s">
+      <c r="P37" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="Q37" s="13" t="s">
+      <c r="Q37" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="R37" s="13" t="s">
+      <c r="R37" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="S37" s="13" t="s">
+      <c r="S37" s="12" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="14" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="14" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="14" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="14" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="14" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="14" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="14" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="14" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2648,23 +2637,23 @@
         <v>205</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>206</v>
+        <v>104</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B68" s="0" t="s">
         <v>207</v>
-      </c>
-      <c r="B68" s="0" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B69" s="0" t="s">
         <v>209</v>
-      </c>
-      <c r="B69" s="0" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2825,22 +2814,6 @@
       </c>
       <c r="B89" s="0" t="s">
         <v>249</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="B90" s="0" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="B91" s="0" t="s">
-        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -2861,17 +2834,17 @@
   </sheetPr>
   <dimension ref="A1:U37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y18" activeCellId="0" sqref="Y18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A42" activeCellId="1" sqref="C43:D43 A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.1133603238866"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="15.7611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.331983805668"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.1174089068826"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.4615384615385"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2891,53 +2864,53 @@
       <c r="E1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="J1" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="L1" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="M1" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="N1" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="O1" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="P1" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="Q1" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="R1" s="0" t="s">
         <v>262</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="S1" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="T1" s="0" t="s">
         <v>264</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="U1" s="0" t="s">
         <v>265</v>
-      </c>
-      <c r="R1" s="0" t="s">
-        <v>266</v>
-      </c>
-      <c r="S1" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="T1" s="0" t="s">
-        <v>268</v>
-      </c>
-      <c r="U1" s="0" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2951,10 +2924,10 @@
         <v>7</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>8</v>
@@ -3010,10 +2983,10 @@
         <v>41</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>10</v>
@@ -3069,10 +3042,10 @@
         <v>17</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>9</v>
@@ -3131,10 +3104,10 @@
         <v>71</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>8</v>
@@ -3196,10 +3169,10 @@
         <v>11</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>8</v>
@@ -3255,10 +3228,10 @@
         <v>49</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>9</v>
@@ -3317,52 +3290,52 @@
         <v>81</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>283</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>285</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>285</v>
+        <v>279</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>281</v>
       </c>
       <c r="L8" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="M8" s="15" t="s">
-        <v>285</v>
-      </c>
-      <c r="N8" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="O8" s="15" t="s">
-        <v>285</v>
-      </c>
-      <c r="P8" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q8" s="15" t="s">
-        <v>285</v>
-      </c>
-      <c r="R8" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="S8" s="15" t="s">
-        <v>285</v>
+      <c r="M8" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q8" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="R8" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="S8" s="16" t="s">
+        <v>281</v>
       </c>
       <c r="T8" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="U8" s="15" t="s">
-        <v>285</v>
+      <c r="U8" s="16" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3382,10 +3355,10 @@
         <v>74</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>9</v>
@@ -3441,10 +3414,10 @@
         <v>34</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>8</v>
@@ -3506,19 +3479,19 @@
         <v>54</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>284</v>
+        <v>287</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>280</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="J11" s="15" t="s">
-        <v>284</v>
+      <c r="J11" s="16" t="s">
+        <v>280</v>
       </c>
       <c r="K11" s="0" t="n">
         <v>22</v>
@@ -3529,20 +3502,20 @@
       <c r="M11" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="N11" s="15" t="s">
-        <v>284</v>
+      <c r="N11" s="16" t="s">
+        <v>280</v>
       </c>
       <c r="O11" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="P11" s="15" t="s">
-        <v>284</v>
+      <c r="P11" s="16" t="s">
+        <v>280</v>
       </c>
       <c r="Q11" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="R11" s="15" t="s">
-        <v>284</v>
+      <c r="R11" s="16" t="s">
+        <v>280</v>
       </c>
       <c r="S11" s="0" t="n">
         <v>22</v>
@@ -3571,10 +3544,10 @@
         <v>28</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>8</v>
@@ -3633,19 +3606,19 @@
         <v>67</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>295</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>296</v>
+        <v>291</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>292</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="J13" s="15" t="s">
-        <v>296</v>
+      <c r="J13" s="16" t="s">
+        <v>292</v>
       </c>
       <c r="K13" s="0" t="n">
         <v>21</v>
@@ -3656,20 +3629,20 @@
       <c r="M13" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="N13" s="15" t="s">
-        <v>296</v>
+      <c r="N13" s="16" t="s">
+        <v>292</v>
       </c>
       <c r="O13" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="P13" s="15" t="s">
-        <v>296</v>
+      <c r="P13" s="16" t="s">
+        <v>292</v>
       </c>
       <c r="Q13" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="R13" s="15" t="s">
-        <v>296</v>
+      <c r="R13" s="16" t="s">
+        <v>292</v>
       </c>
       <c r="S13" s="0" t="n">
         <v>21</v>
@@ -3695,13 +3668,13 @@
         <v>14</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>298</v>
-      </c>
-      <c r="J14" s="15" t="s">
-        <v>284</v>
+        <v>294</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>280</v>
       </c>
       <c r="K14" s="0" t="n">
         <v>22</v>
@@ -3712,20 +3685,20 @@
       <c r="M14" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="N14" s="15" t="s">
-        <v>284</v>
+      <c r="N14" s="16" t="s">
+        <v>280</v>
       </c>
       <c r="O14" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="P14" s="15" t="s">
-        <v>284</v>
+      <c r="P14" s="16" t="s">
+        <v>280</v>
       </c>
       <c r="Q14" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="R14" s="15" t="s">
-        <v>284</v>
+      <c r="R14" s="16" t="s">
+        <v>280</v>
       </c>
       <c r="S14" s="0" t="n">
         <v>22</v>
@@ -3739,7 +3712,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>18</v>
@@ -3754,10 +3727,10 @@
         <v>21</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>9</v>
@@ -3816,57 +3789,57 @@
         <v>77</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>296</v>
-      </c>
-      <c r="I16" s="15" t="s">
-        <v>285</v>
-      </c>
-      <c r="J16" s="15" t="s">
-        <v>296</v>
-      </c>
-      <c r="K16" s="15" t="s">
-        <v>285</v>
-      </c>
-      <c r="L16" s="15" t="s">
-        <v>296</v>
-      </c>
-      <c r="M16" s="15" t="s">
-        <v>285</v>
-      </c>
-      <c r="N16" s="15" t="s">
-        <v>296</v>
-      </c>
-      <c r="O16" s="15" t="s">
-        <v>285</v>
-      </c>
-      <c r="P16" s="15" t="s">
-        <v>296</v>
-      </c>
-      <c r="Q16" s="15" t="s">
-        <v>285</v>
-      </c>
-      <c r="R16" s="15" t="s">
-        <v>296</v>
-      </c>
-      <c r="S16" s="15" t="s">
-        <v>285</v>
-      </c>
-      <c r="T16" s="15" t="s">
-        <v>296</v>
-      </c>
-      <c r="U16" s="15" t="s">
-        <v>285</v>
+        <v>299</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="L16" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="M16" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="N16" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="O16" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="P16" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q16" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="R16" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="S16" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="T16" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="U16" s="16" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>58</v>
@@ -3878,19 +3851,19 @@
         <v>60</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="J17" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="K17" s="15" t="s">
-        <v>307</v>
+      <c r="J17" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="K17" s="16" t="s">
+        <v>303</v>
       </c>
       <c r="L17" s="0" t="n">
         <v>9</v>
@@ -3898,20 +3871,20 @@
       <c r="M17" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="N17" s="15" t="s">
-        <v>284</v>
+      <c r="N17" s="16" t="s">
+        <v>280</v>
       </c>
       <c r="O17" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="P17" s="15" t="s">
-        <v>284</v>
+      <c r="P17" s="16" t="s">
+        <v>280</v>
       </c>
       <c r="Q17" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="R17" s="15" t="s">
-        <v>284</v>
+      <c r="R17" s="16" t="s">
+        <v>280</v>
       </c>
       <c r="S17" s="0" t="n">
         <v>20</v>
@@ -3940,10 +3913,10 @@
         <v>64</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="H18" s="0" t="n">
         <v>8</v>
@@ -3957,8 +3930,8 @@
       <c r="K18" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="L18" s="15" t="s">
-        <v>310</v>
+      <c r="L18" s="16" t="s">
+        <v>306</v>
       </c>
       <c r="M18" s="0" t="n">
         <v>24</v>
@@ -3981,8 +3954,8 @@
       <c r="S18" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="T18" s="15" t="s">
-        <v>310</v>
+      <c r="T18" s="16" t="s">
+        <v>306</v>
       </c>
       <c r="U18" s="0" t="n">
         <v>22</v>
@@ -3993,19 +3966,19 @@
         <v>24</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="H19" s="0" t="n">
         <v>8</v>
@@ -4061,13 +4034,13 @@
         <v>68</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="H20" s="0" t="n">
         <v>8</v>
@@ -4117,19 +4090,19 @@
         <v>51</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="H21" s="0" t="n">
         <v>8</v>
@@ -4179,64 +4152,64 @@
         <v>57</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="H22" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="I22" s="15" t="s">
-        <v>285</v>
+      <c r="I22" s="16" t="s">
+        <v>281</v>
       </c>
       <c r="J22" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="K22" s="15" t="s">
-        <v>285</v>
+      <c r="K22" s="16" t="s">
+        <v>281</v>
       </c>
       <c r="L22" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="M22" s="15" t="s">
-        <v>285</v>
+      <c r="M22" s="16" t="s">
+        <v>281</v>
       </c>
       <c r="N22" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="O22" s="15" t="s">
-        <v>285</v>
+      <c r="O22" s="16" t="s">
+        <v>281</v>
       </c>
       <c r="P22" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="Q22" s="15" t="s">
-        <v>285</v>
+      <c r="Q22" s="16" t="s">
+        <v>281</v>
       </c>
       <c r="R22" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="S22" s="15" t="s">
-        <v>285</v>
+      <c r="S22" s="16" t="s">
+        <v>281</v>
       </c>
       <c r="T22" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="U22" s="15" t="s">
-        <v>285</v>
+      <c r="U22" s="16" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4250,13 +4223,13 @@
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="H23" s="0" t="n">
         <v>8</v>
@@ -4306,22 +4279,22 @@
         <v>36</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="H24" s="0" t="n">
         <v>9</v>
@@ -4356,25 +4329,25 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="H25" s="0" t="n">
         <v>9</v>
@@ -4427,19 +4400,19 @@
         <v>82</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="H26" s="0" t="n">
         <v>8</v>
@@ -4495,21 +4468,21 @@
         <v>86</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>346</v>
-      </c>
-      <c r="H27" s="16" t="n">
-        <v>8</v>
-      </c>
-      <c r="I27" s="16" t="n">
+        <v>342</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="I27" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="J27" s="16" t="n">
-        <v>8</v>
-      </c>
-      <c r="K27" s="16" t="n">
+      <c r="J27" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="K27" s="0" t="n">
         <v>21</v>
       </c>
       <c r="L27" s="0" t="n">
@@ -4518,22 +4491,22 @@
       <c r="M27" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="N27" s="16" t="n">
-        <v>8</v>
-      </c>
-      <c r="O27" s="16" t="n">
+      <c r="N27" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="O27" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="P27" s="16" t="n">
-        <v>8</v>
-      </c>
-      <c r="Q27" s="16" t="n">
+      <c r="P27" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q27" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="R27" s="16" t="n">
-        <v>8</v>
-      </c>
-      <c r="S27" s="16" t="n">
+      <c r="R27" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="S27" s="0" t="n">
         <v>21</v>
       </c>
       <c r="T27" s="0" t="n">
@@ -4557,21 +4530,21 @@
         <v>99</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>348</v>
-      </c>
-      <c r="H28" s="16" t="n">
+        <v>344</v>
+      </c>
+      <c r="H28" s="0" t="n">
         <v>8</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="J28" s="16" t="n">
-        <v>8</v>
-      </c>
-      <c r="K28" s="16" t="n">
+      <c r="J28" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="K28" s="0" t="n">
         <v>21</v>
       </c>
       <c r="L28" s="0" t="n">
@@ -4580,22 +4553,22 @@
       <c r="M28" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="N28" s="16" t="n">
-        <v>8</v>
-      </c>
-      <c r="O28" s="16" t="n">
+      <c r="N28" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="O28" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="P28" s="16" t="n">
-        <v>8</v>
-      </c>
-      <c r="Q28" s="16" t="n">
+      <c r="P28" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q28" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="R28" s="16" t="n">
-        <v>8</v>
-      </c>
-      <c r="S28" s="16" t="n">
+      <c r="R28" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="S28" s="0" t="n">
         <v>21</v>
       </c>
       <c r="T28" s="0" t="n">
@@ -4619,10 +4592,10 @@
         <v>106</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="H29" s="0" t="n">
         <v>9</v>
@@ -4678,10 +4651,10 @@
         <v>111</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="H30" s="0" t="n">
         <v>10</v>
@@ -4740,10 +4713,10 @@
         <v>117</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="H31" s="0" t="n">
         <v>9</v>
@@ -4799,10 +4772,10 @@
         <v>122</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="H32" s="0" t="n">
         <v>10</v>
@@ -4861,10 +4834,10 @@
         <v>128</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="H33" s="0" t="n">
         <v>8</v>
@@ -4920,10 +4893,10 @@
         <v>133</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="H34" s="0" t="n">
         <v>10</v>
@@ -4973,10 +4946,10 @@
         <v>137</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="H35" s="0" t="n">
         <v>9</v>
@@ -5032,10 +5005,10 @@
         <v>142</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="H36" s="0" t="n">
         <v>8</v>
@@ -5088,10 +5061,10 @@
         <v>146</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="H37" s="0" t="n">
         <v>8</v>
@@ -5155,7 +5128,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C43:D43 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>